<commit_message>
Expanding DS page methods
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData1.xlsx
+++ b/src/test/resources/testdata/TestData1.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Default_LoginCredentials" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="DataStructure" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">TestCaseID</t>
   </si>
@@ -38,6 +39,21 @@
   </si>
   <si>
     <t xml:space="preserve">Welcome@01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print("hello");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello</t>
   </si>
 </sst>
 </file>
@@ -151,8 +167,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -191,4 +207,53 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Register and stack updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData1.xlsx
+++ b/src/test/resources/testdata/TestData1.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{ACE48F89-BC96-4358-BF65-7775C9D275F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{372C5935-EEF8-4FC7-A57E-97C767842431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default_LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="3" r:id="rId2"/>
     <sheet name="DataStructure" sheetId="2" r:id="rId3"/>
+    <sheet name="Stack" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:K2"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -128,13 +129,19 @@
   </si>
   <si>
     <t>Welcome/123</t>
+  </si>
+  <si>
+    <t>InvalidCode</t>
+  </si>
+  <si>
+    <t>a=b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -177,6 +184,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -272,6 +284,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2155CF6-E984-4F67-9354-C278C96C8106}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -795,9 +808,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -828,6 +841,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -836,4 +857,46 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13F23F3-1D7E-46C4-9AD1-9453DD6D08F3}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Input code file name change
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData1.xlsx
+++ b/src/test/resources/testdata/TestData1.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{718F8BD0-AC34-459E-BC90-F302C21B8E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BF9756FF-F281-4B85-80F7-BA325962193F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default_LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="DataStructure" sheetId="2" r:id="rId2"/>
     <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Graph" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E9"/>
+  <oleSize ref="A1:I9"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -516,7 +517,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -571,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77EEB37-5FD3-425D-9E8F-E1A2240FEFF9}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
@@ -662,4 +663,57 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653FDF10-7838-46F3-854D-81BF49873BD4}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>